<commit_message>
Adds reference network for US and Canada also there is not sheet for Germany with total traffic matrix
</commit_message>
<xml_diff>
--- a/references/germany/Germany.xlsx
+++ b/references/germany/Germany.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="210" windowWidth="17820" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="210" windowWidth="17820" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Physical" sheetId="1" r:id="rId1"/>
-    <sheet name="IP" sheetId="2" r:id="rId2"/>
-    <sheet name="Voice" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Total" sheetId="5" r:id="rId2"/>
+    <sheet name="IP" sheetId="2" r:id="rId3"/>
+    <sheet name="Voice" sheetId="3" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="23">
   <si>
     <t>B</t>
   </si>
@@ -83,6 +84,9 @@
   </si>
   <si>
     <t>German network transaction data traffic matrix [Gbps]</t>
+  </si>
+  <si>
+    <t>German network total traffic matrix [Gbps]</t>
   </si>
 </sst>
 </file>
@@ -953,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -1457,6 +1461,1037 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="18" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>11.536</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15.85</v>
+      </c>
+      <c r="E3" s="2">
+        <v>17.48</v>
+      </c>
+      <c r="F3" s="2">
+        <v>12.496</v>
+      </c>
+      <c r="G3" s="2">
+        <v>57.834000000000003</v>
+      </c>
+      <c r="H3" s="2">
+        <v>24.835999999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>27.065999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.46</v>
+      </c>
+      <c r="K3" s="2">
+        <v>18.702000000000002</v>
+      </c>
+      <c r="L3" s="2">
+        <v>43.588000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="N3" s="2">
+        <v>19.728000000000002</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>15.811999999999999</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>22.916</v>
+      </c>
+      <c r="R3" s="2">
+        <v>14.204000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.536</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.4459999999999997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8.0280000000000005</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.8179999999999996</v>
+      </c>
+      <c r="G4" s="2">
+        <v>25.687999999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>12.906000000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>13.752000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.35</v>
+      </c>
+      <c r="K4" s="2">
+        <v>8.4879999999999995</v>
+      </c>
+      <c r="L4" s="2">
+        <v>16.192</v>
+      </c>
+      <c r="M4" s="2">
+        <v>4.1479999999999997</v>
+      </c>
+      <c r="N4" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>6.5860000000000003</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>9.7780000000000005</v>
+      </c>
+      <c r="R4" s="2">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15.85</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.4459999999999997</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16.213999999999999</v>
+      </c>
+      <c r="F5" s="2">
+        <v>14.704000000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="H5" s="2">
+        <v>14.635999999999999</v>
+      </c>
+      <c r="I5" s="2">
+        <v>17.257999999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>3.532</v>
+      </c>
+      <c r="K5" s="2">
+        <v>15.981999999999999</v>
+      </c>
+      <c r="L5" s="2">
+        <v>22.815999999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>6.3179999999999996</v>
+      </c>
+      <c r="N5" s="2">
+        <v>11.978</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>9.6479999999999997</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>14.528</v>
+      </c>
+      <c r="R5" s="2">
+        <v>8.8460000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17.48</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8.0280000000000005</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16.213999999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>16.844000000000001</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43.423999999999999</v>
+      </c>
+      <c r="H6" s="2">
+        <v>16.013999999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>18.43</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3.9820000000000002</v>
+      </c>
+      <c r="K6" s="2">
+        <v>24.103999999999999</v>
+      </c>
+      <c r="L6" s="2">
+        <v>25.102</v>
+      </c>
+      <c r="M6" s="2">
+        <v>7.1120000000000001</v>
+      </c>
+      <c r="N6" s="2">
+        <v>13.353999999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>10.708</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>16.277999999999999</v>
+      </c>
+      <c r="R6" s="2">
+        <v>9.8740000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12.496</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.8179999999999996</v>
+      </c>
+      <c r="D7" s="2">
+        <v>14.704000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>16.844000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>31.004000000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>11.504</v>
+      </c>
+      <c r="I7" s="2">
+        <v>13.228</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.8039999999999998</v>
+      </c>
+      <c r="K7" s="2">
+        <v>13.81</v>
+      </c>
+      <c r="L7" s="2">
+        <v>17.95</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5.0060000000000002</v>
+      </c>
+      <c r="N7" s="2">
+        <v>9.4879999999999995</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>7.6159999999999997</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>11.513999999999999</v>
+      </c>
+      <c r="R7" s="2">
+        <v>7.008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>57.834000000000003</v>
+      </c>
+      <c r="C8" s="2">
+        <v>25.687999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>38.909999999999997</v>
+      </c>
+      <c r="E8" s="2">
+        <v>43.423999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>31.004000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>51.491999999999997</v>
+      </c>
+      <c r="I8" s="2">
+        <v>58.223999999999997</v>
+      </c>
+      <c r="J8" s="2">
+        <v>14.484</v>
+      </c>
+      <c r="K8" s="2">
+        <v>47.234000000000002</v>
+      </c>
+      <c r="L8" s="2">
+        <v>82.6</v>
+      </c>
+      <c r="M8" s="2">
+        <v>27.655999999999999</v>
+      </c>
+      <c r="N8" s="2">
+        <v>45.768000000000001</v>
+      </c>
+      <c r="O8" s="2">
+        <v>288.48</v>
+      </c>
+      <c r="P8" s="2">
+        <v>37.692</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>57.36</v>
+      </c>
+      <c r="R8" s="2">
+        <v>34.613999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>24.835999999999999</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12.906000000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>14.635999999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>16.013999999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11.504</v>
+      </c>
+      <c r="G9" s="2">
+        <v>51.491999999999997</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>27.004000000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="K9" s="2">
+        <v>17.018000000000001</v>
+      </c>
+      <c r="L9" s="2">
+        <v>33.942</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8.4719999999999995</v>
+      </c>
+      <c r="N9" s="2">
+        <v>17.021999999999998</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>13.593999999999999</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>20.065999999999999</v>
+      </c>
+      <c r="R9" s="2">
+        <v>12.372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>27.065999999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>13.752000000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>17.257999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>18.43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>13.228</v>
+      </c>
+      <c r="G10" s="2">
+        <v>58.223999999999997</v>
+      </c>
+      <c r="H10" s="2">
+        <v>27.004000000000001</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.4139999999999997</v>
+      </c>
+      <c r="K10" s="2">
+        <v>19.521999999999998</v>
+      </c>
+      <c r="L10" s="2">
+        <v>38.752000000000002</v>
+      </c>
+      <c r="M10" s="2">
+        <v>9.5960000000000001</v>
+      </c>
+      <c r="N10" s="2">
+        <v>18.986000000000001</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>15.343999999999999</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>22.574000000000002</v>
+      </c>
+      <c r="R10" s="2">
+        <v>13.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.46</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.35</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.532</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.9820000000000002</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.8039999999999998</v>
+      </c>
+      <c r="G11" s="2">
+        <v>14.484</v>
+      </c>
+      <c r="H11" s="2">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.4139999999999997</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>4.3460000000000001</v>
+      </c>
+      <c r="L11" s="2">
+        <v>7.9340000000000002</v>
+      </c>
+      <c r="M11" s="2">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="N11" s="2">
+        <v>4.5739999999999998</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3.67</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>7.3440000000000003</v>
+      </c>
+      <c r="R11" s="2">
+        <v>3.6720000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>18.702000000000002</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8.4879999999999995</v>
+      </c>
+      <c r="D12" s="2">
+        <v>15.981999999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>24.103999999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>13.81</v>
+      </c>
+      <c r="G12" s="2">
+        <v>47.234000000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <v>17.018000000000001</v>
+      </c>
+      <c r="I12" s="2">
+        <v>19.521999999999998</v>
+      </c>
+      <c r="J12" s="2">
+        <v>4.3460000000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>26.928000000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>7.8140000000000001</v>
+      </c>
+      <c r="N12" s="2">
+        <v>14.385999999999999</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>11.564</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>17.666</v>
+      </c>
+      <c r="R12" s="2">
+        <v>10.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43.588000000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>16.192</v>
+      </c>
+      <c r="D13" s="2">
+        <v>22.815999999999999</v>
+      </c>
+      <c r="E13" s="2">
+        <v>25.102</v>
+      </c>
+      <c r="F13" s="2">
+        <v>17.95</v>
+      </c>
+      <c r="G13" s="2">
+        <v>82.6</v>
+      </c>
+      <c r="H13" s="2">
+        <v>33.942</v>
+      </c>
+      <c r="I13" s="2">
+        <v>38.752000000000002</v>
+      </c>
+      <c r="J13" s="2">
+        <v>7.9340000000000002</v>
+      </c>
+      <c r="K13" s="2">
+        <v>26.928000000000001</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>13.997999999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <v>28.748000000000001</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>23.722000000000001</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>33.392000000000003</v>
+      </c>
+      <c r="R13" s="2">
+        <v>20.702000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.1479999999999997</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6.3179999999999996</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7.1120000000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5.0060000000000002</v>
+      </c>
+      <c r="G14" s="2">
+        <v>27.655999999999999</v>
+      </c>
+      <c r="H14" s="2">
+        <v>8.4719999999999995</v>
+      </c>
+      <c r="I14" s="2">
+        <v>9.5960000000000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="K14" s="2">
+        <v>7.8140000000000001</v>
+      </c>
+      <c r="L14" s="2">
+        <v>13.997999999999999</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>6.468</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>11.288</v>
+      </c>
+      <c r="R14" s="2">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>19.728000000000002</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="D15" s="2">
+        <v>11.978</v>
+      </c>
+      <c r="E15" s="2">
+        <v>13.353999999999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.4879999999999995</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45.768000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>17.021999999999998</v>
+      </c>
+      <c r="I15" s="2">
+        <v>18.986000000000001</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4.5739999999999998</v>
+      </c>
+      <c r="K15" s="2">
+        <v>14.385999999999999</v>
+      </c>
+      <c r="L15" s="2">
+        <v>28.748000000000001</v>
+      </c>
+      <c r="M15" s="2">
+        <v>7.88</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>14.007999999999999</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>20.065999999999999</v>
+      </c>
+      <c r="R15" s="2">
+        <v>13.638</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>288.48</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15.811999999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6.5860000000000003</v>
+      </c>
+      <c r="D17" s="2">
+        <v>9.6479999999999997</v>
+      </c>
+      <c r="E17" s="2">
+        <v>10.708</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.6159999999999997</v>
+      </c>
+      <c r="G17" s="2">
+        <v>37.692</v>
+      </c>
+      <c r="H17" s="2">
+        <v>13.593999999999999</v>
+      </c>
+      <c r="I17" s="2">
+        <v>15.343999999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>3.67</v>
+      </c>
+      <c r="K17" s="2">
+        <v>11.564</v>
+      </c>
+      <c r="L17" s="2">
+        <v>23.722000000000001</v>
+      </c>
+      <c r="M17" s="2">
+        <v>6.468</v>
+      </c>
+      <c r="N17" s="2">
+        <v>14.007999999999999</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>16.07</v>
+      </c>
+      <c r="R17" s="2">
+        <v>10.154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>22.916</v>
+      </c>
+      <c r="C18" s="2">
+        <v>9.7780000000000005</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14.528</v>
+      </c>
+      <c r="E18" s="2">
+        <v>16.277999999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>11.513999999999999</v>
+      </c>
+      <c r="G18" s="2">
+        <v>57.36</v>
+      </c>
+      <c r="H18" s="2">
+        <v>20.065999999999999</v>
+      </c>
+      <c r="I18" s="2">
+        <v>22.574000000000002</v>
+      </c>
+      <c r="J18" s="2">
+        <v>7.3440000000000003</v>
+      </c>
+      <c r="K18" s="2">
+        <v>17.666</v>
+      </c>
+      <c r="L18" s="2">
+        <v>33.392000000000003</v>
+      </c>
+      <c r="M18" s="2">
+        <v>11.288</v>
+      </c>
+      <c r="N18" s="2">
+        <v>20.065999999999999</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>16.07</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0</v>
+      </c>
+      <c r="R18" s="2">
+        <v>18.056000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>14.204000000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8.8460000000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9.8740000000000006</v>
+      </c>
+      <c r="F19" s="2">
+        <v>7.008</v>
+      </c>
+      <c r="G19" s="2">
+        <v>34.613999999999997</v>
+      </c>
+      <c r="H19" s="2">
+        <v>12.372</v>
+      </c>
+      <c r="I19" s="2">
+        <v>13.86</v>
+      </c>
+      <c r="J19" s="2">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="K19" s="2">
+        <v>10.67</v>
+      </c>
+      <c r="L19" s="2">
+        <v>20.702000000000002</v>
+      </c>
+      <c r="M19" s="2">
+        <v>6.16</v>
+      </c>
+      <c r="N19" s="2">
+        <v>13.638</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>10.154</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>18.056000000000001</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -2483,7 +3518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
@@ -3514,11 +4549,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>